<commit_message>
Submit TST786 ,TST495 ,TST1327,TST569
</commit_message>
<xml_diff>
--- a/NformTester/NformTester/Keywordscripts/TST1104_ExportActionHistoryForDeviceAlarms.xlsx
+++ b/NformTester/NformTester/Keywordscripts/TST1104_ExportActionHistoryForDeviceAlarms.xlsx
@@ -1260,7 +1260,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7908" uniqueCount="884">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7907" uniqueCount="883">
   <si>
     <t>FormLogin_to_LiebertR_Nform</t>
   </si>
@@ -3937,9 +3937,6 @@
   </si>
   <si>
     <t>Equal</t>
-  </si>
-  <si>
-    <t>45-66</t>
   </si>
   <si>
     <t>Enabled</t>
@@ -4582,8 +4579,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O156"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F34" workbookViewId="0">
-      <selection activeCell="I55" sqref="I55"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4816,9 +4813,7 @@
       <c r="A8" s="2" t="s">
         <v>847</v>
       </c>
-      <c r="B8" s="6" t="s">
-        <v>882</v>
-      </c>
+      <c r="B8" s="6"/>
       <c r="C8" s="3">
         <v>7</v>
       </c>
@@ -6002,7 +5997,7 @@
         <v>7</v>
       </c>
       <c r="H53" s="21" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="I53" s="3" t="s">
         <v>881</v>
@@ -6032,7 +6027,7 @@
         <v>7</v>
       </c>
       <c r="H54" s="21" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="I54" s="3" t="s">
         <v>881</v>

</xml_diff>